<commit_message>
Dieu Thuong dien roi
</commit_message>
<xml_diff>
--- a/Project estimation (1).xlsx
+++ b/Project estimation (1).xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17030"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\44K223.02\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="390" yWindow="555" windowWidth="19815" windowHeight="9405" activeTab="1"/>
   </bookViews>
@@ -15,7 +20,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'PROJECT PLAN'!$A$7:$H$59</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -430,7 +435,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
     <numFmt numFmtId="165" formatCode="d/m/yyyy"/>
@@ -981,6 +986,45 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -996,12 +1040,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1013,39 +1051,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1063,6 +1068,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -4386,8 +4394,8 @@
   </sheetPr>
   <dimension ref="A1:AC1014"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="F64" sqref="F64"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E68" sqref="E68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -4556,7 +4564,7 @@
       <c r="E8" s="53"/>
       <c r="F8" s="53">
         <f>SUM(F9:F16)</f>
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="G8" s="55">
         <v>44284</v>
@@ -4588,7 +4596,7 @@
     </row>
     <row r="9" spans="1:29" ht="15">
       <c r="A9" s="56"/>
-      <c r="B9" s="108" t="s">
+      <c r="B9" s="97" t="s">
         <v>87</v>
       </c>
       <c r="C9" s="57" t="s">
@@ -4600,7 +4608,9 @@
       <c r="E9" s="57" t="s">
         <v>90</v>
       </c>
-      <c r="F9" s="58"/>
+      <c r="F9" s="58">
+        <v>10</v>
+      </c>
       <c r="G9" s="59"/>
       <c r="H9" s="60"/>
       <c r="I9" s="4"/>
@@ -4610,7 +4620,7 @@
     </row>
     <row r="10" spans="1:29" ht="15">
       <c r="A10" s="58"/>
-      <c r="B10" s="109"/>
+      <c r="B10" s="98"/>
       <c r="C10" s="57" t="s">
         <v>26</v>
       </c>
@@ -4632,7 +4642,7 @@
     </row>
     <row r="11" spans="1:29" ht="15">
       <c r="A11" s="58"/>
-      <c r="B11" s="109"/>
+      <c r="B11" s="98"/>
       <c r="C11" s="57" t="s">
         <v>20</v>
       </c>
@@ -4652,7 +4662,7 @@
     </row>
     <row r="12" spans="1:29" ht="15">
       <c r="A12" s="58"/>
-      <c r="B12" s="110"/>
+      <c r="B12" s="99"/>
       <c r="C12" s="57" t="s">
         <v>21</v>
       </c>
@@ -4672,7 +4682,7 @@
     </row>
     <row r="13" spans="1:29" ht="15">
       <c r="A13" s="58"/>
-      <c r="B13" s="111" t="s">
+      <c r="B13" s="101" t="s">
         <v>88</v>
       </c>
       <c r="C13" s="57" t="s">
@@ -4694,7 +4704,7 @@
     </row>
     <row r="14" spans="1:29" ht="15">
       <c r="A14" s="58"/>
-      <c r="B14" s="112"/>
+      <c r="B14" s="102"/>
       <c r="C14" s="57" t="s">
         <v>19</v>
       </c>
@@ -4716,7 +4726,7 @@
     </row>
     <row r="15" spans="1:29" ht="15">
       <c r="A15" s="58"/>
-      <c r="B15" s="112"/>
+      <c r="B15" s="102"/>
       <c r="C15" s="57" t="s">
         <v>89</v>
       </c>
@@ -4738,7 +4748,7 @@
     </row>
     <row r="16" spans="1:29" ht="15">
       <c r="A16" s="58"/>
-      <c r="B16" s="113"/>
+      <c r="B16" s="103"/>
       <c r="C16" s="57" t="s">
         <v>25</v>
       </c>
@@ -4771,7 +4781,7 @@
       <c r="E17" s="53"/>
       <c r="F17" s="53">
         <f>SUM(F18:F25)</f>
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="G17" s="55">
         <v>44291</v>
@@ -4803,7 +4813,7 @@
     </row>
     <row r="18" spans="1:29" ht="15">
       <c r="A18" s="58"/>
-      <c r="B18" s="111" t="s">
+      <c r="B18" s="101" t="s">
         <v>96</v>
       </c>
       <c r="C18" s="57" t="s">
@@ -4827,7 +4837,7 @@
     </row>
     <row r="19" spans="1:29" ht="15">
       <c r="A19" s="58"/>
-      <c r="B19" s="113"/>
+      <c r="B19" s="103"/>
       <c r="C19" s="57" t="s">
         <v>98</v>
       </c>
@@ -4847,7 +4857,7 @@
     </row>
     <row r="20" spans="1:29" ht="15">
       <c r="A20" s="56"/>
-      <c r="B20" s="108" t="s">
+      <c r="B20" s="97" t="s">
         <v>97</v>
       </c>
       <c r="C20" s="57" t="s">
@@ -4871,7 +4881,7 @@
     </row>
     <row r="21" spans="1:29" ht="15">
       <c r="A21" s="58"/>
-      <c r="B21" s="109"/>
+      <c r="B21" s="98"/>
       <c r="C21" s="57" t="s">
         <v>29</v>
       </c>
@@ -4893,7 +4903,7 @@
     </row>
     <row r="22" spans="1:29" ht="15">
       <c r="A22" s="58"/>
-      <c r="B22" s="109"/>
+      <c r="B22" s="98"/>
       <c r="C22" s="63" t="s">
         <v>30</v>
       </c>
@@ -4913,7 +4923,7 @@
     </row>
     <row r="23" spans="1:29" s="46" customFormat="1" ht="15">
       <c r="A23" s="58"/>
-      <c r="B23" s="109"/>
+      <c r="B23" s="98"/>
       <c r="C23" s="63" t="s">
         <v>99</v>
       </c>
@@ -4935,7 +4945,7 @@
     </row>
     <row r="24" spans="1:29" s="46" customFormat="1" ht="15">
       <c r="A24" s="58"/>
-      <c r="B24" s="109"/>
+      <c r="B24" s="98"/>
       <c r="C24" s="63" t="s">
         <v>100</v>
       </c>
@@ -4945,7 +4955,9 @@
       <c r="E24" s="65" t="s">
         <v>90</v>
       </c>
-      <c r="F24" s="64"/>
+      <c r="F24" s="64">
+        <v>9</v>
+      </c>
       <c r="G24" s="62"/>
       <c r="H24" s="62"/>
       <c r="I24" s="5"/>
@@ -4955,7 +4967,7 @@
     </row>
     <row r="25" spans="1:29" s="46" customFormat="1" ht="15">
       <c r="A25" s="58"/>
-      <c r="B25" s="110"/>
+      <c r="B25" s="99"/>
       <c r="C25" s="63" t="s">
         <v>101</v>
       </c>
@@ -4988,7 +5000,7 @@
       <c r="E26" s="53"/>
       <c r="F26" s="53">
         <f>SUM(F27:F39)</f>
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="G26" s="55">
         <v>44298</v>
@@ -5020,7 +5032,7 @@
     </row>
     <row r="27" spans="1:29" ht="15">
       <c r="A27" s="58"/>
-      <c r="B27" s="114" t="s">
+      <c r="B27" s="93" t="s">
         <v>102</v>
       </c>
       <c r="C27" s="57" t="s">
@@ -5032,7 +5044,9 @@
       <c r="E27" s="57" t="s">
         <v>90</v>
       </c>
-      <c r="F27" s="58"/>
+      <c r="F27" s="58">
+        <v>9</v>
+      </c>
       <c r="G27" s="60"/>
       <c r="H27" s="59"/>
       <c r="I27" s="4"/>
@@ -5042,7 +5056,7 @@
     </row>
     <row r="28" spans="1:29" ht="15">
       <c r="A28" s="67"/>
-      <c r="B28" s="116"/>
+      <c r="B28" s="100"/>
       <c r="C28" s="57" t="s">
         <v>105</v>
       </c>
@@ -5064,7 +5078,7 @@
     </row>
     <row r="29" spans="1:29" ht="15">
       <c r="A29" s="58"/>
-      <c r="B29" s="116"/>
+      <c r="B29" s="100"/>
       <c r="C29" s="57" t="s">
         <v>106</v>
       </c>
@@ -5084,7 +5098,7 @@
     </row>
     <row r="30" spans="1:29" ht="15">
       <c r="A30" s="68"/>
-      <c r="B30" s="116"/>
+      <c r="B30" s="100"/>
       <c r="C30" s="57" t="s">
         <v>107</v>
       </c>
@@ -5106,7 +5120,7 @@
     </row>
     <row r="31" spans="1:29" ht="15">
       <c r="A31" s="68"/>
-      <c r="B31" s="115"/>
+      <c r="B31" s="94"/>
       <c r="C31" s="57" t="s">
         <v>108</v>
       </c>
@@ -5126,7 +5140,7 @@
     </row>
     <row r="32" spans="1:29" ht="15">
       <c r="A32" s="58"/>
-      <c r="B32" s="114" t="s">
+      <c r="B32" s="93" t="s">
         <v>38</v>
       </c>
       <c r="C32" s="57" t="s">
@@ -5148,7 +5162,7 @@
     </row>
     <row r="33" spans="1:29" ht="15">
       <c r="A33" s="58"/>
-      <c r="B33" s="116"/>
+      <c r="B33" s="100"/>
       <c r="C33" s="57" t="s">
         <v>109</v>
       </c>
@@ -5170,7 +5184,7 @@
     </row>
     <row r="34" spans="1:29" s="46" customFormat="1" ht="15">
       <c r="A34" s="58"/>
-      <c r="B34" s="115"/>
+      <c r="B34" s="94"/>
       <c r="C34" s="57" t="s">
         <v>110</v>
       </c>
@@ -5192,7 +5206,7 @@
     </row>
     <row r="35" spans="1:29" s="46" customFormat="1" ht="15">
       <c r="A35" s="58"/>
-      <c r="B35" s="114" t="s">
+      <c r="B35" s="93" t="s">
         <v>103</v>
       </c>
       <c r="C35" s="57" t="s">
@@ -5216,7 +5230,7 @@
     </row>
     <row r="36" spans="1:29" s="46" customFormat="1" ht="15">
       <c r="A36" s="58"/>
-      <c r="B36" s="115"/>
+      <c r="B36" s="94"/>
       <c r="C36" s="57" t="s">
         <v>37</v>
       </c>
@@ -5236,7 +5250,7 @@
     </row>
     <row r="37" spans="1:29" s="46" customFormat="1" ht="15">
       <c r="A37" s="58"/>
-      <c r="B37" s="111" t="s">
+      <c r="B37" s="101" t="s">
         <v>104</v>
       </c>
       <c r="C37" s="57" t="s">
@@ -5260,7 +5274,7 @@
     </row>
     <row r="38" spans="1:29" s="46" customFormat="1" ht="15">
       <c r="A38" s="58"/>
-      <c r="B38" s="112"/>
+      <c r="B38" s="102"/>
       <c r="C38" s="57" t="s">
         <v>112</v>
       </c>
@@ -5282,7 +5296,7 @@
     </row>
     <row r="39" spans="1:29" s="46" customFormat="1" ht="15">
       <c r="A39" s="58"/>
-      <c r="B39" s="113"/>
+      <c r="B39" s="103"/>
       <c r="C39" s="57" t="s">
         <v>36</v>
       </c>
@@ -5292,7 +5306,9 @@
       <c r="E39" s="57" t="s">
         <v>90</v>
       </c>
-      <c r="F39" s="58"/>
+      <c r="F39" s="58">
+        <v>2</v>
+      </c>
       <c r="G39" s="60"/>
       <c r="H39" s="59"/>
       <c r="I39" s="5"/>
@@ -5313,7 +5329,7 @@
       <c r="E40" s="53"/>
       <c r="F40" s="53">
         <f>SUM(F41:F48)</f>
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="G40" s="55">
         <v>44305</v>
@@ -5345,7 +5361,7 @@
     </row>
     <row r="41" spans="1:29" ht="17.25" customHeight="1">
       <c r="A41" s="58"/>
-      <c r="B41" s="114" t="s">
+      <c r="B41" s="93" t="s">
         <v>113</v>
       </c>
       <c r="C41" s="57" t="s">
@@ -5357,7 +5373,9 @@
       <c r="E41" s="57" t="s">
         <v>90</v>
       </c>
-      <c r="F41" s="58"/>
+      <c r="F41" s="58">
+        <v>6</v>
+      </c>
       <c r="G41" s="62"/>
       <c r="H41" s="62"/>
       <c r="I41" s="4"/>
@@ -5367,7 +5385,7 @@
     </row>
     <row r="42" spans="1:29" ht="15">
       <c r="A42" s="67"/>
-      <c r="B42" s="115"/>
+      <c r="B42" s="94"/>
       <c r="C42" s="57" t="s">
         <v>116</v>
       </c>
@@ -5389,7 +5407,7 @@
     </row>
     <row r="43" spans="1:29" ht="15">
       <c r="A43" s="58"/>
-      <c r="B43" s="114" t="s">
+      <c r="B43" s="93" t="s">
         <v>114</v>
       </c>
       <c r="C43" s="57" t="s">
@@ -5413,7 +5431,7 @@
     </row>
     <row r="44" spans="1:29" ht="15">
       <c r="A44" s="68"/>
-      <c r="B44" s="115"/>
+      <c r="B44" s="94"/>
       <c r="C44" s="57" t="s">
         <v>117</v>
       </c>
@@ -5433,7 +5451,7 @@
     </row>
     <row r="45" spans="1:29" ht="15">
       <c r="A45" s="68"/>
-      <c r="B45" s="93" t="s">
+      <c r="B45" s="108" t="s">
         <v>115</v>
       </c>
       <c r="C45" s="57" t="s">
@@ -5455,7 +5473,7 @@
     </row>
     <row r="46" spans="1:29" s="46" customFormat="1" ht="15">
       <c r="A46" s="68"/>
-      <c r="B46" s="94"/>
+      <c r="B46" s="109"/>
       <c r="C46" s="57" t="s">
         <v>118</v>
       </c>
@@ -5475,7 +5493,7 @@
     </row>
     <row r="47" spans="1:29" s="46" customFormat="1" ht="15">
       <c r="A47" s="68"/>
-      <c r="B47" s="94"/>
+      <c r="B47" s="109"/>
       <c r="C47" s="57" t="s">
         <v>119</v>
       </c>
@@ -5497,7 +5515,7 @@
     </row>
     <row r="48" spans="1:29" s="46" customFormat="1" ht="15">
       <c r="A48" s="68"/>
-      <c r="B48" s="95"/>
+      <c r="B48" s="110"/>
       <c r="C48" s="57" t="s">
         <v>120</v>
       </c>
@@ -5530,7 +5548,7 @@
       <c r="E49" s="53"/>
       <c r="F49" s="53">
         <f>SUM(F50:F58)</f>
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="G49" s="55">
         <v>44312</v>
@@ -5562,7 +5580,7 @@
     </row>
     <row r="50" spans="1:29" ht="15">
       <c r="A50" s="58"/>
-      <c r="B50" s="96" t="s">
+      <c r="B50" s="111" t="s">
         <v>121</v>
       </c>
       <c r="C50" s="57" t="s">
@@ -5574,7 +5592,9 @@
       <c r="E50" s="58" t="s">
         <v>90</v>
       </c>
-      <c r="F50" s="58"/>
+      <c r="F50" s="58">
+        <v>10</v>
+      </c>
       <c r="G50" s="60"/>
       <c r="H50" s="60"/>
       <c r="I50" s="4"/>
@@ -5584,7 +5604,7 @@
     </row>
     <row r="51" spans="1:29" ht="15">
       <c r="A51" s="58"/>
-      <c r="B51" s="97"/>
+      <c r="B51" s="112"/>
       <c r="C51" s="57" t="s">
         <v>125</v>
       </c>
@@ -5606,7 +5626,7 @@
     </row>
     <row r="52" spans="1:29" ht="15">
       <c r="A52" s="68"/>
-      <c r="B52" s="98" t="s">
+      <c r="B52" s="95" t="s">
         <v>131</v>
       </c>
       <c r="C52" s="57" t="s">
@@ -5628,7 +5648,7 @@
     </row>
     <row r="53" spans="1:29" s="47" customFormat="1" ht="15">
       <c r="A53" s="68"/>
-      <c r="B53" s="99"/>
+      <c r="B53" s="96"/>
       <c r="C53" s="57" t="s">
         <v>133</v>
       </c>
@@ -5650,7 +5670,7 @@
     </row>
     <row r="54" spans="1:29" ht="15">
       <c r="A54" s="68"/>
-      <c r="B54" s="98" t="s">
+      <c r="B54" s="95" t="s">
         <v>122</v>
       </c>
       <c r="C54" s="57" t="s">
@@ -5674,7 +5694,7 @@
     </row>
     <row r="55" spans="1:29" ht="15">
       <c r="A55" s="67"/>
-      <c r="B55" s="99"/>
+      <c r="B55" s="96"/>
       <c r="C55" s="69" t="s">
         <v>127</v>
       </c>
@@ -5690,7 +5710,7 @@
     </row>
     <row r="56" spans="1:29" ht="15">
       <c r="A56" s="67"/>
-      <c r="B56" s="100" t="s">
+      <c r="B56" s="113" t="s">
         <v>123</v>
       </c>
       <c r="C56" s="69" t="s">
@@ -5711,7 +5731,7 @@
     </row>
     <row r="57" spans="1:29" ht="15">
       <c r="A57" s="67"/>
-      <c r="B57" s="101"/>
+      <c r="B57" s="114"/>
       <c r="C57" s="69" t="s">
         <v>74</v>
       </c>
@@ -5730,7 +5750,7 @@
     </row>
     <row r="58" spans="1:29" ht="15">
       <c r="A58" s="67"/>
-      <c r="B58" s="102"/>
+      <c r="B58" s="115"/>
       <c r="C58" s="69" t="s">
         <v>128</v>
       </c>
@@ -5746,18 +5766,18 @@
       <c r="I58" s="22"/>
     </row>
     <row r="59" spans="1:29" ht="15">
-      <c r="A59" s="103" t="s">
+      <c r="A59" s="116" t="s">
         <v>130</v>
       </c>
-      <c r="B59" s="103"/>
-      <c r="C59" s="103"/>
+      <c r="B59" s="116"/>
+      <c r="C59" s="116"/>
       <c r="D59" s="91">
         <f>SUM(D8,D17,D26,D40,D49)</f>
         <v>305</v>
       </c>
       <c r="F59" s="46">
         <f>SUM(F8,F17,F26,F40,F49)</f>
-        <v>143</v>
+        <v>189</v>
       </c>
       <c r="H59" s="22"/>
       <c r="I59" s="22"/>
@@ -5849,7 +5869,9 @@
       <c r="D67" s="71">
         <v>48</v>
       </c>
-      <c r="E67" s="67"/>
+      <c r="E67" s="67">
+        <v>46</v>
+      </c>
       <c r="H67" s="22"/>
       <c r="I67" s="22"/>
     </row>
@@ -10591,6 +10613,14 @@
   </sheetData>
   <autoFilter ref="A7:H59"/>
   <mergeCells count="18">
+    <mergeCell ref="B54:B55"/>
+    <mergeCell ref="B56:B58"/>
+    <mergeCell ref="A59:C59"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="B9:B12"/>
+    <mergeCell ref="B13:B16"/>
+    <mergeCell ref="B18:B19"/>
     <mergeCell ref="B41:B42"/>
     <mergeCell ref="B43:B44"/>
     <mergeCell ref="B52:B53"/>
@@ -10599,16 +10629,8 @@
     <mergeCell ref="B32:B34"/>
     <mergeCell ref="B35:B36"/>
     <mergeCell ref="B37:B39"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="B9:B12"/>
-    <mergeCell ref="B13:B16"/>
-    <mergeCell ref="B18:B19"/>
     <mergeCell ref="B45:B48"/>
     <mergeCell ref="B50:B51"/>
-    <mergeCell ref="B54:B55"/>
-    <mergeCell ref="B56:B58"/>
-    <mergeCell ref="A59:C59"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>